<commit_message>
Aggiunto secondo tasto Resource 2, modifiche al primo
Il codice è creato e generato con touch GFX, importato
in CubeIDE, non è stato ulteriormente toccato o aggiornato.

Il codice relativo al tasto 1 che non ha un corrispettivo
per il tasto 2 era stato aggiunto a mano, il resto
è il codice di base dal quale sviluppare per generare l'azione
richiesta
</commit_message>
<xml_diff>
--- a/SampleProject/TouchGFX/assets/texts/texts.xlsx
+++ b/SampleProject/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="53">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -168,6 +168,12 @@
   </si>
   <si>
     <t xml:space="preserve">Main Menu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resource 2</t>
   </si>
 </sst>
 </file>
@@ -1662,6 +1668,23 @@
         <v>50</v>
       </c>
     </row>
+    <row r="6">
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Added a settings menu and interaction in touchGFX
After that code was rigenerated.
</commit_message>
<xml_diff>
--- a/SampleProject/TouchGFX/assets/texts/texts.xlsx
+++ b/SampleProject/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="55">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -174,6 +174,12 @@
   </si>
   <si>
     <t xml:space="preserve">Resource 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Settings Menu</t>
   </si>
 </sst>
 </file>
@@ -1685,6 +1691,23 @@
         <v>52</v>
       </c>
     </row>
+    <row r="7">
+      <c r="B7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>